<commit_message>
CSV file import implemented
</commit_message>
<xml_diff>
--- a/spec/factories/Diseases_new.xlsx
+++ b/spec/factories/Diseases_new.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -28,31 +28,28 @@
     <t xml:space="preserve">Symptons</t>
   </si>
   <si>
-    <t xml:space="preserve">CueDis_6</t>
+    <t xml:space="preserve">CueDis_19</t>
   </si>
   <si>
     <t xml:space="preserve">Unexpected weight loss, night sweats, or fever</t>
   </si>
   <si>
-    <t xml:space="preserve">CueDis_7</t>
+    <t xml:space="preserve">CueDis_20</t>
   </si>
   <si>
     <t xml:space="preserve">a condition that impairs the body's ability to process blood glucose</t>
   </si>
   <si>
-    <t xml:space="preserve">CueDis_8</t>
+    <t xml:space="preserve">CueDis_21</t>
   </si>
   <si>
     <t xml:space="preserve">urgency to go to the toilet, frequent passing of loose, watery faeces</t>
   </si>
   <si>
-    <t xml:space="preserve">CueDis_9</t>
+    <t xml:space="preserve">CueDis_22</t>
   </si>
   <si>
     <t xml:space="preserve">chronic tiredness or sleepiness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CueDis_10</t>
   </si>
 </sst>
 </file>
@@ -185,14 +182,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,11 +232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
diseases controller upload method spec done
</commit_message>
<xml_diff>
--- a/spec/factories/Diseases_new.xlsx
+++ b/spec/factories/Diseases_new.xlsx
@@ -28,25 +28,25 @@
     <t xml:space="preserve">Symptons</t>
   </si>
   <si>
-    <t xml:space="preserve">CueDis_19</t>
+    <t xml:space="preserve">spec123</t>
   </si>
   <si>
     <t xml:space="preserve">Unexpected weight loss, night sweats, or fever</t>
   </si>
   <si>
-    <t xml:space="preserve">CueDis_20</t>
+    <t xml:space="preserve">spec124</t>
   </si>
   <si>
     <t xml:space="preserve">a condition that impairs the body's ability to process blood glucose</t>
   </si>
   <si>
-    <t xml:space="preserve">CueDis_21</t>
+    <t xml:space="preserve">spec125</t>
   </si>
   <si>
     <t xml:space="preserve">urgency to go to the toilet, frequent passing of loose, watery faeces</t>
   </si>
   <si>
-    <t xml:space="preserve">CueDis_22</t>
+    <t xml:space="preserve">spec126</t>
   </si>
   <si>
     <t xml:space="preserve">chronic tiredness or sleepiness</t>
@@ -182,14 +182,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>